<commit_message>
API Gateway ZUUL Implementation
</commit_message>
<xml_diff>
--- a/MicroservicesTools.xlsx
+++ b/MicroservicesTools.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Microservices Frameworks" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="74">
   <si>
     <t>Registration,  Discovery, Configuration, Monitoring</t>
   </si>
@@ -352,6 +352,9 @@
     <t>For generating multiple instance  we also use following attributes in application.properties file.
 eureka.instance.instanceId=${spring.application.name}:${random.value}
 server.port=0   (dynamically assign port)</t>
+  </si>
+  <si>
+    <t>Just add the dependency in the pom.xml for referring a config server</t>
   </si>
 </sst>
 </file>
@@ -968,7 +971,7 @@
       </c>
       <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>53</v>
       </c>
@@ -1004,7 +1007,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1131,10 +1134,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1176,6 +1179,11 @@
       </c>
       <c r="B5" s="1" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>